<commit_message>
Changes in main results
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\OneDrive\Dokumente\Sc_Master\Masterthesis\Project\DomAdapt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4679B-7C4A-4358-91E4-44C253A3E4CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04749B6C-A43D-40E7-8DBC-F88E18B87521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{C35B19F6-04BE-4ADE-8625-8B0ABD47C8B3}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C35B19F6-04BE-4ADE-8625-8B0ABD47C8B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -543,6 +543,98 @@
   </si>
   <si>
     <t>5fold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train MLP </t>
+  </si>
+  <si>
+    <t>Train MLP0 with adaptive pooling, dropout 0.1</t>
+  </si>
+  <si>
+    <t>due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change activation function to sigmoid. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Train MLP with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>architecture2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on  50% of simulations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Train MLP with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>architecture4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on  50% of simulations</t>
+    </r>
+  </si>
+  <si>
+    <t>ms2sims</t>
+  </si>
+  <si>
+    <t>Model Selection on Simulations</t>
+  </si>
+  <si>
+    <t>Select Model architecture for pretraining on 10% of Simulations</t>
+  </si>
+  <si>
+    <t>Train MLP0 with adaptive_pooling (architecture3) and dropout 0.0, 0.1, 0.2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">output: grid_search/simulations. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Architecture5</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -610,10 +702,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0397FBB-D2CD-440A-BC03-013EBB84CD2B}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,7 +2190,7 @@
         <v>128</v>
       </c>
       <c r="J38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2128,7 +2216,7 @@
         <v>129</v>
       </c>
       <c r="J39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2235,7 +2323,7 @@
         <v>139</v>
       </c>
       <c r="J43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K43" t="s">
         <v>140</v>
@@ -2267,7 +2355,7 @@
         <v>142</v>
       </c>
       <c r="J44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2293,7 +2381,7 @@
         <v>143</v>
       </c>
       <c r="J45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2322,7 +2410,7 @@
         <v>144</v>
       </c>
       <c r="J46" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="K46" t="s">
         <v>145</v>
@@ -2354,7 +2442,252 @@
         <v>147</v>
       </c>
       <c r="J47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="6">
+        <v>7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>57</v>
+      </c>
+      <c r="H48" t="s">
+        <v>161</v>
+      </c>
+      <c r="J48" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="D49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="6">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" t="s">
+        <v>157</v>
+      </c>
+      <c r="J50" t="s">
+        <v>158</v>
+      </c>
+      <c r="K50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="6">
+        <v>8</v>
+      </c>
+      <c r="G51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H51" t="s">
+        <v>160</v>
+      </c>
+      <c r="J51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>44147</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="D52" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="6">
+        <v>8</v>
+      </c>
+      <c r="G52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52" t="s">
+        <v>161</v>
+      </c>
+      <c r="J52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D53" t="s">
+        <v>163</v>
+      </c>
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="6">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" t="s">
+        <v>164</v>
+      </c>
+      <c r="J53" t="s">
+        <v>55</v>
+      </c>
+      <c r="K53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D54" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="6">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J54" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D55" t="s">
+        <v>163</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="6">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>162</v>
+      </c>
+      <c r="H55" t="s">
+        <v>164</v>
+      </c>
+      <c r="J55" t="s">
+        <v>55</v>
+      </c>
+      <c r="K55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>44148</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D56" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="6">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>162</v>
+      </c>
+      <c r="H56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J56" t="s">
+        <v>55</v>
+      </c>
+      <c r="K56" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2367,7 +2700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCE0804-6847-4A20-B6B7-E620D3B0F445}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>